<commit_message>
update test case, data, test script
</commit_message>
<xml_diff>
--- a/data/dataLogin.xlsx
+++ b/data/dataLogin.xlsx
@@ -1,33 +1,95 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27932"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Testing\RobotFramework\LibQNU\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F04A871-A127-45A1-8C7D-3184FE3517C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="24975" windowHeight="10155" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="5580" yWindow="3600" windowWidth="17280" windowHeight="9465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="152511" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+  <si>
+    <t>${data_login_cardnum}</t>
+  </si>
+  <si>
+    <t>${data_login_password}</t>
+  </si>
+  <si>
+    <t>4451190019zxc</t>
+  </si>
+  <si>
+    <t>123@$Sxzz</t>
+  </si>
+  <si>
+    <t>4451190019</t>
+  </si>
+  <si>
+    <t>${patron_name}</t>
+  </si>
+  <si>
+    <t>Cao Nguyễn Xuân Huy</t>
+  </si>
+  <si>
+    <t>Số thẻ hoặc mật khẩu không hợp lệ !</t>
+  </si>
+  <si>
+    <t>${MSG_ALERT_LOGIN_CONTENT}</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -42,84 +104,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -166,7 +173,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -201,7 +208,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -376,28 +383,126 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>4451190019</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4451190019</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>4451190019</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE764F9-8913-4003-9B09-3772D669816D}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>4451190019</v>
+      </c>
+      <c r="B2" s="1">
+        <v>4451190019</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
not sure about language
</commit_message>
<xml_diff>
--- a/data/dataLogin.xlsx
+++ b/data/dataLogin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Testing\RobotFramework\LibQNU\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F04A871-A127-45A1-8C7D-3184FE3517C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9849E2BF-CFF3-41CB-9D06-2A55B2339516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="3600" windowWidth="17280" windowHeight="9465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11370" yWindow="5985" windowWidth="17280" windowHeight="9465" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -390,8 +390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -468,7 +468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE764F9-8913-4003-9B09-3772D669816D}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>